<commit_message>
Fixed all mode and acc_phon and utt_ level LMEMs
</commit_message>
<xml_diff>
--- a/Ch_7_Sentence_Modes/Excel/Utterance Phonetic Models.xlsx
+++ b/Ch_7_Sentence_Modes/Excel/Utterance Phonetic Models.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoi\Github\PhD\Ch_7_Sentence_Modes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoi\Github\PhD\Ch_7_Sentence_Modes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308B9EED-6CD1-4C44-9F5B-FEA13E193ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E3E0CC-393F-4CD9-8FCC-737827769EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5F934F14-35FB-48F8-B9CC-AA2F647F3C27}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>MDC</t>
   </si>
@@ -147,6 +147,9 @@
       </rPr>
       <t>c</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
   </si>
 </sst>
 </file>
@@ -485,14 +488,34 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="78">
+  <dxfs count="113">
+    <dxf>
+      <font>
+        <color rgb="FFD95F02"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
         <color rgb="FFD95F02"/>
       </font>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -500,7 +523,7 @@
         <i val="0"/>
         <color rgb="FF1B9E77"/>
       </font>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -508,7 +531,6 @@
         <i val="0"/>
         <color rgb="FF1B9E77"/>
       </font>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -517,51 +539,6 @@
         <color rgb="FF1B9E77"/>
       </font>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD95F02"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD95F02"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -723,6 +700,11 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFD95F02"/>
       </font>
     </dxf>
@@ -774,6 +756,11 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFD95F02"/>
       </font>
     </dxf>
@@ -975,6 +962,241 @@
         <color rgb="FF1B9E77"/>
       </font>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD95F02"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFD95F02"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD95F02"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFD95F02"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD95F02"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFD95F02"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFD95F02"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD95F02"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD95F02"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1207,16 +1429,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.37</c:v>
+                    <c:v>1.5</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.7150000000000003</c:v>
+                    <c:v>2.1139999999999999</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.298</c:v>
+                    <c:v>1.228</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.0570000000000004</c:v>
+                    <c:v>2.214</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1228,16 +1450,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.37</c:v>
+                    <c:v>1.5</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.7150000000000003</c:v>
+                    <c:v>2.1139999999999999</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.298</c:v>
+                    <c:v>1.228</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.0570000000000004</c:v>
+                    <c:v>2.214</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1280,16 +1502,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-0.42</c:v>
+                  <c:v>-1.694</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.8439999999999999</c:v>
+                  <c:v>-3.7210000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.12</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0960000000000001</c:v>
+                  <c:v>4.6859999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1359,7 +1581,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
-          <c:min val="-5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1691,16 +1912,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2.9699999999999989</c:v>
+                    <c:v>2.208999999999989</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.6500000000000057</c:v>
+                    <c:v>1.921999999999997</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.7179999999999893</c:v>
+                    <c:v>2.0889999999999986</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.117999999999995</c:v>
+                    <c:v>2.5789999999999935</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1712,16 +1933,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2.9699999999999989</c:v>
+                    <c:v>2.208999999999989</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.6500000000000057</c:v>
+                    <c:v>1.921999999999997</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.7179999999999893</c:v>
+                    <c:v>2.0889999999999986</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.117999999999995</c:v>
+                    <c:v>2.5789999999999935</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1764,16 +1985,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>86.081999999999994</c:v>
+                  <c:v>89.230999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>86.551000000000002</c:v>
+                  <c:v>89.652000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86.840999999999994</c:v>
+                  <c:v>90.016999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88.369</c:v>
+                  <c:v>91.546999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2671,11 +2892,14 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="slope_b0"/>
+      <sheetName val="utt_f0_b0"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="1">
+          <cell r="A1" t="str">
+            <v>intercept</v>
+          </cell>
           <cell r="B1" t="str">
             <v>estimate</v>
           </cell>
@@ -2689,7 +2913,7 @@
             <v>97.5% CI</v>
           </cell>
           <cell r="F1" t="str">
-            <v>t.value</v>
+            <v>z.value</v>
           </cell>
           <cell r="G1" t="str">
             <v>df</v>
@@ -2698,123 +2922,138 @@
             <v>p.value</v>
           </cell>
           <cell r="I1" t="str">
-            <v>p.adj. (bf=4)</v>
+            <v>p.adj (BH)</v>
           </cell>
           <cell r="J1" t="str">
-            <v xml:space="preserve">signif. </v>
+            <v>signif.</v>
           </cell>
         </row>
         <row r="2">
+          <cell r="A2" t="str">
+            <v>modeMDC</v>
+          </cell>
           <cell r="B2">
-            <v>-0.42</v>
+            <v>89.230999999999995</v>
           </cell>
           <cell r="C2">
-            <v>0.69899999999999995</v>
+            <v>1.127</v>
           </cell>
           <cell r="D2">
-            <v>-1.79</v>
+            <v>87.022000000000006</v>
           </cell>
           <cell r="E2">
-            <v>0.94899999999999995</v>
+            <v>91.44</v>
           </cell>
           <cell r="F2">
-            <v>-0.60199999999999998</v>
+            <v>79.168999999999997</v>
           </cell>
           <cell r="G2">
-            <v>9.9700000000000006</v>
+            <v>11.69</v>
           </cell>
           <cell r="H2">
-            <v>0.56079999999999997</v>
+            <v>2.5500000000000001E-17</v>
           </cell>
           <cell r="I2">
-            <v>0.99990000000000001</v>
+            <v>2.0400000000000001E-16</v>
+          </cell>
+          <cell r="J2" t="str">
+            <v>p&lt;0.0001</v>
           </cell>
         </row>
         <row r="3">
+          <cell r="A3" t="str">
+            <v>modeMWH</v>
+          </cell>
           <cell r="B3">
-            <v>-2.8439999999999999</v>
+            <v>89.652000000000001</v>
           </cell>
           <cell r="C3">
-            <v>0.875</v>
+            <v>0.98099999999999998</v>
           </cell>
           <cell r="D3">
-            <v>-4.5590000000000002</v>
+            <v>87.73</v>
           </cell>
           <cell r="E3">
-            <v>-1.129</v>
+            <v>91.573999999999998</v>
           </cell>
           <cell r="F3">
-            <v>-3.25</v>
+            <v>91.424999999999997</v>
           </cell>
           <cell r="G3">
-            <v>9.99</v>
+            <v>10.119999999999999</v>
           </cell>
           <cell r="H3">
-            <v>8.6999999999999994E-3</v>
+            <v>4.28E-16</v>
           </cell>
           <cell r="I3">
-            <v>3.49E-2</v>
+            <v>2.57E-15</v>
           </cell>
           <cell r="J3" t="str">
-            <v>p&lt;0.05</v>
+            <v>p&lt;0.0001</v>
           </cell>
         </row>
         <row r="4">
+          <cell r="A4" t="str">
+            <v>modeMYN</v>
+          </cell>
           <cell r="B4">
-            <v>3.12</v>
+            <v>90.016999999999996</v>
           </cell>
           <cell r="C4">
-            <v>0.66200000000000003</v>
+            <v>1.0660000000000001</v>
           </cell>
           <cell r="D4">
-            <v>1.8220000000000001</v>
+            <v>87.927999999999997</v>
           </cell>
           <cell r="E4">
-            <v>4.4169999999999998</v>
+            <v>92.106999999999999</v>
           </cell>
           <cell r="F4">
-            <v>4.7130000000000001</v>
+            <v>84.435000000000002</v>
           </cell>
           <cell r="G4">
-            <v>10.029999999999999</v>
+            <v>11.53</v>
           </cell>
           <cell r="H4">
-            <v>8.1840999999999999E-4</v>
+            <v>1.86E-17</v>
           </cell>
           <cell r="I4">
-            <v>3.3E-3</v>
+            <v>2.0400000000000001E-16</v>
           </cell>
           <cell r="J4" t="str">
-            <v>p&lt;0.01</v>
+            <v>p&lt;0.0001</v>
           </cell>
         </row>
         <row r="5">
+          <cell r="A5" t="str">
+            <v>modeMDQ</v>
+          </cell>
           <cell r="B5">
-            <v>6.0960000000000001</v>
+            <v>91.546999999999997</v>
           </cell>
           <cell r="C5">
-            <v>1.0489999999999999</v>
+            <v>1.3160000000000001</v>
           </cell>
           <cell r="D5">
-            <v>4.0389999999999997</v>
+            <v>88.968000000000004</v>
           </cell>
           <cell r="E5">
-            <v>8.1530000000000005</v>
+            <v>94.126000000000005</v>
           </cell>
           <cell r="F5">
-            <v>5.8090000000000002</v>
+            <v>69.561999999999998</v>
           </cell>
           <cell r="G5">
-            <v>10.039999999999999</v>
+            <v>12.73</v>
           </cell>
           <cell r="H5">
-            <v>1.6829E-4</v>
+            <v>8.2800000000000006E-18</v>
           </cell>
           <cell r="I5">
-            <v>6.7299999999999999E-4</v>
+            <v>1.99E-16</v>
           </cell>
           <cell r="J5" t="str">
-            <v>p&lt;0.001</v>
+            <v>p&lt;0.0001</v>
           </cell>
         </row>
       </sheetData>
@@ -2827,7 +3066,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="slope_b1"/>
+      <sheetName val="utt_slope_b0"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -2836,241 +3075,144 @@
             <v>intercept</v>
           </cell>
           <cell r="B1" t="str">
-            <v>slope</v>
+            <v>estimate</v>
           </cell>
           <cell r="C1" t="str">
-            <v>estimate</v>
+            <v>std.error</v>
           </cell>
           <cell r="D1" t="str">
-            <v>std.error</v>
+            <v>2.5% CI</v>
           </cell>
           <cell r="E1" t="str">
-            <v>2.5% CI</v>
+            <v>97.5% CI</v>
           </cell>
           <cell r="F1" t="str">
-            <v>97.5% CI</v>
+            <v>z.value</v>
           </cell>
           <cell r="G1" t="str">
-            <v>t.value</v>
+            <v>df</v>
           </cell>
           <cell r="H1" t="str">
-            <v>df</v>
+            <v>p.value</v>
           </cell>
           <cell r="I1" t="str">
-            <v>p.value</v>
+            <v>p.adj (BH)</v>
           </cell>
           <cell r="J1" t="str">
-            <v>p.adj. (bf=4)</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v xml:space="preserve">signif. </v>
+            <v>signif.</v>
           </cell>
         </row>
         <row r="2">
-          <cell r="A2" t="str">
-            <v>modeMDC</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>modeMWH</v>
+          <cell r="B2">
+            <v>-1.694</v>
           </cell>
           <cell r="C2">
-            <v>-2.423</v>
+            <v>0.76500000000000001</v>
           </cell>
           <cell r="D2">
-            <v>1.2310000000000001</v>
+            <v>-3.194</v>
           </cell>
           <cell r="E2">
-            <v>-4.835</v>
+            <v>-0.19400000000000001</v>
           </cell>
           <cell r="F2">
-            <v>-1.2E-2</v>
+            <v>-2.2130000000000001</v>
           </cell>
           <cell r="G2">
-            <v>-1.9690000000000001</v>
+            <v>13.41</v>
           </cell>
           <cell r="H2">
-            <v>9.99</v>
+            <v>4.48E-2</v>
           </cell>
           <cell r="I2">
-            <v>7.7200000000000005E-2</v>
-          </cell>
-          <cell r="J2">
-            <v>0.30890000000000001</v>
+            <v>5.3800000000000001E-2</v>
           </cell>
         </row>
         <row r="3">
-          <cell r="A3" t="str">
-            <v>modeMDC</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>modeMYN</v>
+          <cell r="B3">
+            <v>-3.7210000000000001</v>
           </cell>
           <cell r="C3">
-            <v>3.54</v>
+            <v>1.0780000000000001</v>
           </cell>
           <cell r="D3">
-            <v>0.874</v>
+            <v>-5.835</v>
           </cell>
           <cell r="E3">
-            <v>1.827</v>
+            <v>-1.6080000000000001</v>
           </cell>
           <cell r="F3">
-            <v>5.2530000000000001</v>
+            <v>-3.4510000000000001</v>
           </cell>
           <cell r="G3">
-            <v>4.05</v>
+            <v>9.61</v>
           </cell>
           <cell r="H3">
-            <v>10.01</v>
+            <v>6.6E-3</v>
           </cell>
           <cell r="I3">
-            <v>2.3E-3</v>
-          </cell>
-          <cell r="J3">
-            <v>9.2999999999999992E-3</v>
-          </cell>
-          <cell r="K3" t="str">
-            <v>p&lt;0.01</v>
+            <v>1.18E-2</v>
+          </cell>
+          <cell r="J3" t="str">
+            <v>p&lt;0.05</v>
           </cell>
         </row>
         <row r="4">
-          <cell r="A4" t="str">
-            <v>modeMDC</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>modeMDQ</v>
+          <cell r="B4">
+            <v>1.7</v>
           </cell>
           <cell r="C4">
-            <v>6.516</v>
+            <v>0.627</v>
           </cell>
           <cell r="D4">
-            <v>1.131</v>
+            <v>0.47199999999999998</v>
           </cell>
           <cell r="E4">
-            <v>4.2990000000000004</v>
+            <v>2.9289999999999998</v>
           </cell>
           <cell r="F4">
-            <v>8.7330000000000005</v>
+            <v>2.7130000000000001</v>
           </cell>
           <cell r="G4">
-            <v>5.7610000000000001</v>
+            <v>10.58</v>
           </cell>
           <cell r="H4">
-            <v>10.09</v>
+            <v>2.0799999999999999E-2</v>
           </cell>
           <cell r="I4">
-            <v>1.7642999999999999E-4</v>
-          </cell>
-          <cell r="J4">
-            <v>7.0600000000000003E-4</v>
-          </cell>
-          <cell r="K4" t="str">
-            <v>p&lt;0.001</v>
+            <v>2.7799999999999998E-2</v>
+          </cell>
+          <cell r="J4" t="str">
+            <v>p&lt;0.05</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="A5" t="str">
-            <v>modeMWH</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>modeMYN</v>
+          <cell r="B5">
+            <v>4.6859999999999999</v>
           </cell>
           <cell r="C5">
-            <v>5.9640000000000004</v>
+            <v>1.129</v>
           </cell>
           <cell r="D5">
-            <v>1.417</v>
+            <v>2.472</v>
           </cell>
           <cell r="E5">
-            <v>3.1859999999999999</v>
+            <v>6.899</v>
           </cell>
           <cell r="F5">
-            <v>8.7420000000000009</v>
+            <v>4.149</v>
           </cell>
           <cell r="G5">
-            <v>4.2080000000000002</v>
+            <v>12.74</v>
           </cell>
           <cell r="H5">
-            <v>10.01</v>
+            <v>1.1999999999999999E-3</v>
           </cell>
           <cell r="I5">
-            <v>1.8E-3</v>
-          </cell>
-          <cell r="J5">
-            <v>7.1999999999999998E-3</v>
-          </cell>
-          <cell r="K5" t="str">
+            <v>2.8999999999999998E-3</v>
+          </cell>
+          <cell r="J5" t="str">
             <v>p&lt;0.01</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>modeMWH</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>modeMDQ</v>
-          </cell>
-          <cell r="C6">
-            <v>8.94</v>
-          </cell>
-          <cell r="D6">
-            <v>1.7509999999999999</v>
-          </cell>
-          <cell r="E6">
-            <v>5.508</v>
-          </cell>
-          <cell r="F6">
-            <v>12.372</v>
-          </cell>
-          <cell r="G6">
-            <v>5.1050000000000004</v>
-          </cell>
-          <cell r="H6">
-            <v>10.02</v>
-          </cell>
-          <cell r="I6">
-            <v>4.5785999999999998E-4</v>
-          </cell>
-          <cell r="J6">
-            <v>1.8E-3</v>
-          </cell>
-          <cell r="K6" t="str">
-            <v>p&lt;0.01</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>modeMYN</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>modeMDQ</v>
-          </cell>
-          <cell r="C7">
-            <v>2.976</v>
-          </cell>
-          <cell r="D7">
-            <v>0.79900000000000004</v>
-          </cell>
-          <cell r="E7">
-            <v>1.411</v>
-          </cell>
-          <cell r="F7">
-            <v>4.5419999999999998</v>
-          </cell>
-          <cell r="G7">
-            <v>3.726</v>
-          </cell>
-          <cell r="H7">
-            <v>9.8800000000000008</v>
-          </cell>
-          <cell r="I7">
-            <v>4.0000000000000001E-3</v>
-          </cell>
-          <cell r="J7">
-            <v>1.61E-2</v>
-          </cell>
-          <cell r="K7" t="str">
-            <v>p&lt;0.05</v>
           </cell>
         </row>
       </sheetData>
@@ -3083,7 +3225,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="f0_b0"/>
+      <sheetName val="utt_f0_b1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -3092,159 +3234,238 @@
             <v>intercept</v>
           </cell>
           <cell r="B1" t="str">
+            <v>slope</v>
+          </cell>
+          <cell r="C1" t="str">
             <v>estimate</v>
           </cell>
-          <cell r="C1" t="str">
+          <cell r="D1" t="str">
             <v>std.error</v>
           </cell>
-          <cell r="D1" t="str">
+          <cell r="E1" t="str">
             <v>2.5% CI</v>
           </cell>
-          <cell r="E1" t="str">
+          <cell r="F1" t="str">
             <v>97.5% CI</v>
           </cell>
-          <cell r="F1" t="str">
-            <v>t.value</v>
-          </cell>
           <cell r="G1" t="str">
+            <v>z.value</v>
+          </cell>
+          <cell r="H1" t="str">
             <v>df</v>
           </cell>
-          <cell r="H1" t="str">
+          <cell r="I1" t="str">
             <v>p.value</v>
           </cell>
-          <cell r="I1" t="str">
-            <v>p.adj. (bf=4)</v>
-          </cell>
           <cell r="J1" t="str">
-            <v xml:space="preserve">signif. </v>
+            <v>p.adj (BH)</v>
+          </cell>
+          <cell r="K1" t="str">
+            <v>signif.</v>
           </cell>
         </row>
         <row r="2">
           <cell r="A2" t="str">
             <v>modeMDC</v>
           </cell>
-          <cell r="B2">
-            <v>86.081999999999994</v>
+          <cell r="B2" t="str">
+            <v>modeMWH</v>
           </cell>
           <cell r="C2">
-            <v>1.5149999999999999</v>
+            <v>0.42099999999999999</v>
           </cell>
           <cell r="D2">
-            <v>83.111999999999995</v>
+            <v>0.312</v>
           </cell>
           <cell r="E2">
-            <v>89.052000000000007</v>
+            <v>-0.191</v>
           </cell>
           <cell r="F2">
-            <v>56.805</v>
+            <v>1.0329999999999999</v>
           </cell>
           <cell r="G2">
-            <v>10</v>
+            <v>1.349</v>
           </cell>
           <cell r="H2">
-            <v>6.9199999999999998E-14</v>
+            <v>10.8</v>
           </cell>
           <cell r="I2">
-            <v>2.7699999999999998E-13</v>
-          </cell>
-          <cell r="J2" t="str">
-            <v>p&lt;0.001</v>
+            <v>0.2051</v>
+          </cell>
+          <cell r="J2">
+            <v>0.214</v>
           </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
-            <v>modeMWH</v>
-          </cell>
-          <cell r="B3">
-            <v>86.551000000000002</v>
+            <v>modeMDC</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>modeMYN</v>
           </cell>
           <cell r="C3">
-            <v>1.3520000000000001</v>
+            <v>0.78600000000000003</v>
           </cell>
           <cell r="D3">
-            <v>83.900999999999996</v>
+            <v>0.25</v>
           </cell>
           <cell r="E3">
-            <v>89.200999999999993</v>
+            <v>0.29599999999999999</v>
           </cell>
           <cell r="F3">
-            <v>64.013000000000005</v>
+            <v>1.2769999999999999</v>
           </cell>
           <cell r="G3">
-            <v>10</v>
+            <v>3.1419999999999999</v>
           </cell>
           <cell r="H3">
-            <v>2.1027E-14</v>
+            <v>10.37</v>
           </cell>
           <cell r="I3">
-            <v>8.4100000000000003E-14</v>
-          </cell>
-          <cell r="J3" t="str">
-            <v>p&lt;0.001</v>
+            <v>0.01</v>
+          </cell>
+          <cell r="J3">
+            <v>1.5100000000000001E-2</v>
+          </cell>
+          <cell r="K3" t="str">
+            <v>p&lt;0.05</v>
           </cell>
         </row>
         <row r="4">
           <cell r="A4" t="str">
-            <v>modeMYN</v>
-          </cell>
-          <cell r="B4">
-            <v>86.840999999999994</v>
+            <v>modeMDC</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>modeMDQ</v>
           </cell>
           <cell r="C4">
-            <v>1.387</v>
+            <v>2.3159999999999998</v>
           </cell>
           <cell r="D4">
-            <v>84.123000000000005</v>
+            <v>0.442</v>
           </cell>
           <cell r="E4">
-            <v>89.56</v>
+            <v>1.4490000000000001</v>
           </cell>
           <cell r="F4">
-            <v>62.616</v>
+            <v>3.1829999999999998</v>
           </cell>
           <cell r="G4">
-            <v>10</v>
+            <v>5.2370000000000001</v>
           </cell>
           <cell r="H4">
-            <v>2.6189E-14</v>
+            <v>10.17</v>
           </cell>
           <cell r="I4">
-            <v>1.0499999999999999E-13</v>
-          </cell>
-          <cell r="J4" t="str">
-            <v>p&lt;0.001</v>
+            <v>3.6000000000000002E-4</v>
+          </cell>
+          <cell r="J4">
+            <v>1.1999999999999999E-3</v>
+          </cell>
+          <cell r="K4" t="str">
+            <v>p&lt;0.01</v>
           </cell>
         </row>
         <row r="5">
           <cell r="A5" t="str">
+            <v>modeMWH</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>modeMYN</v>
+          </cell>
+          <cell r="C5">
+            <v>0.36499999999999999</v>
+          </cell>
+          <cell r="D5">
+            <v>0.26700000000000002</v>
+          </cell>
+          <cell r="E5">
+            <v>-0.158</v>
+          </cell>
+          <cell r="F5">
+            <v>0.88900000000000001</v>
+          </cell>
+          <cell r="G5">
+            <v>1.3680000000000001</v>
+          </cell>
+          <cell r="H5">
+            <v>12.73</v>
+          </cell>
+          <cell r="I5">
+            <v>0.1951</v>
+          </cell>
+          <cell r="J5">
+            <v>0.21290000000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>modeMWH</v>
+          </cell>
+          <cell r="B6" t="str">
             <v>modeMDQ</v>
           </cell>
-          <cell r="B5">
-            <v>88.369</v>
-          </cell>
-          <cell r="C5">
-            <v>1.591</v>
-          </cell>
-          <cell r="D5">
-            <v>85.251000000000005</v>
-          </cell>
-          <cell r="E5">
-            <v>91.486999999999995</v>
-          </cell>
-          <cell r="F5">
-            <v>55.555</v>
-          </cell>
-          <cell r="G5">
-            <v>10</v>
-          </cell>
-          <cell r="H5">
-            <v>8.6136E-14</v>
-          </cell>
-          <cell r="I5">
-            <v>3.4499999999999999E-13</v>
-          </cell>
-          <cell r="J5" t="str">
-            <v>p&lt;0.001</v>
+          <cell r="C6">
+            <v>1.8959999999999999</v>
+          </cell>
+          <cell r="D6">
+            <v>0.63900000000000001</v>
+          </cell>
+          <cell r="E6">
+            <v>0.64400000000000002</v>
+          </cell>
+          <cell r="F6">
+            <v>3.1469999999999998</v>
+          </cell>
+          <cell r="G6">
+            <v>2.968</v>
+          </cell>
+          <cell r="H6">
+            <v>10.51</v>
+          </cell>
+          <cell r="I6">
+            <v>1.34E-2</v>
+          </cell>
+          <cell r="J6">
+            <v>1.89E-2</v>
+          </cell>
+          <cell r="K6" t="str">
+            <v>p&lt;0.05</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>modeMYN</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>modeMDQ</v>
+          </cell>
+          <cell r="C7">
+            <v>1.53</v>
+          </cell>
+          <cell r="D7">
+            <v>0.58799999999999997</v>
+          </cell>
+          <cell r="E7">
+            <v>0.377</v>
+          </cell>
+          <cell r="F7">
+            <v>2.6829999999999998</v>
+          </cell>
+          <cell r="G7">
+            <v>2.6019999999999999</v>
+          </cell>
+          <cell r="H7">
+            <v>10.050000000000001</v>
+          </cell>
+          <cell r="I7">
+            <v>2.63E-2</v>
+          </cell>
+          <cell r="J7">
+            <v>3.32E-2</v>
+          </cell>
+          <cell r="K7" t="str">
+            <v>p&lt;0.05</v>
           </cell>
         </row>
       </sheetData>
@@ -3257,244 +3478,18 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="f0_b1"/>
+      <sheetName val="utt_f0_r2"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>intercept</v>
-          </cell>
-          <cell r="B1" t="str">
-            <v>slope</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>estimate</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>std.error</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>2.5% CI</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>97.5% CI</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>t.value</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>df</v>
-          </cell>
-          <cell r="I1" t="str">
-            <v>p.value</v>
-          </cell>
-          <cell r="J1" t="str">
-            <v>p.adj. (bf=4)</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v xml:space="preserve">signif. </v>
-          </cell>
-        </row>
         <row r="2">
-          <cell r="A2" t="str">
-            <v>modeMDC</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>modeMWH</v>
-          </cell>
-          <cell r="C2">
-            <v>0.47</v>
-          </cell>
-          <cell r="D2">
-            <v>0.311</v>
-          </cell>
-          <cell r="E2">
-            <v>-0.13900000000000001</v>
-          </cell>
-          <cell r="F2">
-            <v>1.0780000000000001</v>
-          </cell>
-          <cell r="G2">
-            <v>1.5129999999999999</v>
-          </cell>
-          <cell r="H2">
-            <v>10.07</v>
-          </cell>
-          <cell r="I2">
-            <v>0.16109999999999999</v>
-          </cell>
-          <cell r="J2">
-            <v>0.64439999999999997</v>
+          <cell r="B2">
+            <v>0.94231623989217705</v>
           </cell>
         </row>
         <row r="3">
-          <cell r="A3" t="str">
-            <v>modeMDC</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>modeMYN</v>
-          </cell>
-          <cell r="C3">
-            <v>0.76</v>
-          </cell>
-          <cell r="D3">
-            <v>0.249</v>
-          </cell>
-          <cell r="E3">
-            <v>0.27200000000000002</v>
-          </cell>
-          <cell r="F3">
-            <v>1.2470000000000001</v>
-          </cell>
-          <cell r="G3">
-            <v>3.0510000000000002</v>
-          </cell>
-          <cell r="H3">
-            <v>10.07</v>
-          </cell>
-          <cell r="I3">
-            <v>1.21E-2</v>
-          </cell>
-          <cell r="J3">
-            <v>4.8500000000000001E-2</v>
-          </cell>
-          <cell r="K3" t="str">
-            <v>p&lt;0.05</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>modeMDC</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>modeMDQ</v>
-          </cell>
-          <cell r="C4">
-            <v>2.2869999999999999</v>
-          </cell>
-          <cell r="D4">
-            <v>0.438</v>
-          </cell>
-          <cell r="E4">
-            <v>1.4279999999999999</v>
-          </cell>
-          <cell r="F4">
-            <v>3.1469999999999998</v>
-          </cell>
-          <cell r="G4">
-            <v>5.2160000000000002</v>
-          </cell>
-          <cell r="H4">
-            <v>10.06</v>
-          </cell>
-          <cell r="I4">
-            <v>3.8405999999999998E-4</v>
-          </cell>
-          <cell r="J4">
-            <v>1.5E-3</v>
-          </cell>
-          <cell r="K4" t="str">
-            <v>p&lt;0.01</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>modeMWH</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>modeMYN</v>
-          </cell>
-          <cell r="C5">
-            <v>0.28999999999999998</v>
-          </cell>
-          <cell r="D5">
-            <v>0.252</v>
-          </cell>
-          <cell r="E5">
-            <v>-0.20499999999999999</v>
-          </cell>
-          <cell r="F5">
-            <v>0.78500000000000003</v>
-          </cell>
-          <cell r="G5">
-            <v>1.1479999999999999</v>
-          </cell>
-          <cell r="H5">
-            <v>9.98</v>
-          </cell>
-          <cell r="I5">
-            <v>0.27760000000000001</v>
-          </cell>
-          <cell r="J5">
-            <v>0.99990000000000001</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>modeMWH</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>modeMDQ</v>
-          </cell>
-          <cell r="C6">
-            <v>1.8169999999999999</v>
-          </cell>
-          <cell r="D6">
-            <v>0.63200000000000001</v>
-          </cell>
-          <cell r="E6">
-            <v>0.57999999999999996</v>
-          </cell>
-          <cell r="F6">
-            <v>3.0550000000000002</v>
-          </cell>
-          <cell r="G6">
-            <v>2.8780000000000001</v>
-          </cell>
-          <cell r="H6">
-            <v>10.039999999999999</v>
-          </cell>
-          <cell r="I6">
-            <v>1.6400000000000001E-2</v>
-          </cell>
-          <cell r="J6">
-            <v>6.5600000000000006E-2</v>
-          </cell>
-          <cell r="K6" t="str">
-            <v>(p&lt;0.1)</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>modeMYN</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>modeMDQ</v>
-          </cell>
-          <cell r="C7">
-            <v>1.528</v>
-          </cell>
-          <cell r="D7">
-            <v>0.59099999999999997</v>
-          </cell>
-          <cell r="E7">
-            <v>0.37</v>
-          </cell>
-          <cell r="F7">
-            <v>2.6859999999999999</v>
-          </cell>
-          <cell r="G7">
-            <v>2.585</v>
-          </cell>
-          <cell r="H7">
-            <v>10.06</v>
-          </cell>
-          <cell r="I7">
-            <v>2.7099999999999999E-2</v>
-          </cell>
-          <cell r="J7">
-            <v>0.1082</v>
+          <cell r="B3">
+            <v>0.52849012129538697</v>
           </cell>
         </row>
       </sheetData>
@@ -3507,18 +3502,18 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="f0_r2"/>
+      <sheetName val="utt_slope_r2"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>0.94762073814392001</v>
+            <v>0.83641134398527495</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>2.8174816408763698E-2</v>
+            <v>0.51029969546325904</v>
           </cell>
         </row>
       </sheetData>
@@ -3531,18 +3526,250 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="slope_r2"/>
+      <sheetName val="utt_slope_b1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>intercept</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>slope</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>estimate</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>std.error</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>2.5% CI</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>97.5% CI</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>z.value</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>df</v>
+          </cell>
+          <cell r="I1" t="str">
+            <v>p.value</v>
+          </cell>
+          <cell r="J1" t="str">
+            <v>p.adj (BH)</v>
+          </cell>
+          <cell r="K1" t="str">
+            <v>signif.</v>
+          </cell>
+        </row>
         <row r="2">
-          <cell r="B2">
-            <v>0.80018328350564605</v>
+          <cell r="A2" t="str">
+            <v>modeMDC</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>modeMWH</v>
+          </cell>
+          <cell r="C2">
+            <v>-2.028</v>
+          </cell>
+          <cell r="D2">
+            <v>1.234</v>
+          </cell>
+          <cell r="E2">
+            <v>-4.4470000000000001</v>
+          </cell>
+          <cell r="F2">
+            <v>0.39200000000000002</v>
+          </cell>
+          <cell r="G2">
+            <v>-1.643</v>
+          </cell>
+          <cell r="H2">
+            <v>10.15</v>
+          </cell>
+          <cell r="I2">
+            <v>0.13100000000000001</v>
+          </cell>
+          <cell r="J2">
+            <v>0.14979999999999999</v>
           </cell>
         </row>
         <row r="3">
-          <cell r="B3">
-            <v>0.48829263568562897</v>
+          <cell r="A3" t="str">
+            <v>modeMDC</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>modeMYN</v>
+          </cell>
+          <cell r="C3">
+            <v>3.3940000000000001</v>
+          </cell>
+          <cell r="D3">
+            <v>0.8</v>
+          </cell>
+          <cell r="E3">
+            <v>1.825</v>
+          </cell>
+          <cell r="F3">
+            <v>4.9630000000000001</v>
+          </cell>
+          <cell r="G3">
+            <v>4.24</v>
+          </cell>
+          <cell r="H3">
+            <v>10.02</v>
+          </cell>
+          <cell r="I3">
+            <v>1.6999999999999999E-3</v>
+          </cell>
+          <cell r="J3">
+            <v>3.7000000000000002E-3</v>
+          </cell>
+          <cell r="K3" t="str">
+            <v>p&lt;0.01</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>modeMDC</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>modeMDQ</v>
+          </cell>
+          <cell r="C4">
+            <v>6.38</v>
+          </cell>
+          <cell r="D4">
+            <v>1.1180000000000001</v>
+          </cell>
+          <cell r="E4">
+            <v>4.1890000000000001</v>
+          </cell>
+          <cell r="F4">
+            <v>8.57</v>
+          </cell>
+          <cell r="G4">
+            <v>5.7089999999999996</v>
+          </cell>
+          <cell r="H4">
+            <v>10.119999999999999</v>
+          </cell>
+          <cell r="I4">
+            <v>1.8699999999999999E-4</v>
+          </cell>
+          <cell r="J4">
+            <v>8.9999999999999998E-4</v>
+          </cell>
+          <cell r="K4" t="str">
+            <v>p&lt;0.001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>modeMWH</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>modeMYN</v>
+          </cell>
+          <cell r="C5">
+            <v>5.4219999999999997</v>
+          </cell>
+          <cell r="D5">
+            <v>1.4370000000000001</v>
+          </cell>
+          <cell r="E5">
+            <v>2.6059999999999999</v>
+          </cell>
+          <cell r="F5">
+            <v>8.2379999999999995</v>
+          </cell>
+          <cell r="G5">
+            <v>3.7730000000000001</v>
+          </cell>
+          <cell r="H5">
+            <v>10.26</v>
+          </cell>
+          <cell r="I5">
+            <v>3.5000000000000001E-3</v>
+          </cell>
+          <cell r="J5">
+            <v>7.0000000000000001E-3</v>
+          </cell>
+          <cell r="K5" t="str">
+            <v>p&lt;0.01</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>modeMWH</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>modeMDQ</v>
+          </cell>
+          <cell r="C6">
+            <v>8.407</v>
+          </cell>
+          <cell r="D6">
+            <v>1.796</v>
+          </cell>
+          <cell r="E6">
+            <v>4.8860000000000001</v>
+          </cell>
+          <cell r="F6">
+            <v>11.928000000000001</v>
+          </cell>
+          <cell r="G6">
+            <v>4.68</v>
+          </cell>
+          <cell r="H6">
+            <v>10.199999999999999</v>
+          </cell>
+          <cell r="I6">
+            <v>8.2200000000000003E-4</v>
+          </cell>
+          <cell r="J6">
+            <v>2.2000000000000001E-3</v>
+          </cell>
+          <cell r="K6" t="str">
+            <v>p&lt;0.01</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>modeMYN</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>modeMDQ</v>
+          </cell>
+          <cell r="C7">
+            <v>2.9849999999999999</v>
+          </cell>
+          <cell r="D7">
+            <v>0.876</v>
+          </cell>
+          <cell r="E7">
+            <v>1.268</v>
+          </cell>
+          <cell r="F7">
+            <v>4.7030000000000003</v>
+          </cell>
+          <cell r="G7">
+            <v>3.4060000000000001</v>
+          </cell>
+          <cell r="H7">
+            <v>9.83</v>
+          </cell>
+          <cell r="I7">
+            <v>6.8999999999999999E-3</v>
+          </cell>
+          <cell r="J7">
+            <v>1.18E-2</v>
+          </cell>
+          <cell r="K7" t="str">
+            <v>p&lt;0.05</v>
           </cell>
         </row>
       </sheetData>
@@ -3850,7 +4077,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA75D8A-458C-4EF4-8CA5-966D1B6FEE89}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3887,46 +4116,46 @@
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:11" s="10" customFormat="1" ht="25.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="25.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="str">
-        <f>RIGHT([3]f0_b0!A1,3)</f>
-        <v>ept</v>
+        <f>[1]utt_f0_b0!A1</f>
+        <v>intercept</v>
       </c>
       <c r="B2" s="8" t="str">
-        <f>[3]f0_b0!B1</f>
+        <f>[1]utt_f0_b0!B1</f>
         <v>estimate</v>
       </c>
       <c r="C2" s="8" t="str">
-        <f>[3]f0_b0!C1</f>
+        <f>[1]utt_f0_b0!C1</f>
         <v>std.error</v>
       </c>
       <c r="D2" s="8" t="str">
-        <f>[3]f0_b0!D1</f>
+        <f>[1]utt_f0_b0!D1</f>
         <v>2.5% CI</v>
       </c>
       <c r="E2" s="8" t="str">
-        <f>[3]f0_b0!E1</f>
+        <f>[1]utt_f0_b0!E1</f>
         <v>97.5% CI</v>
       </c>
       <c r="F2" s="8" t="str">
-        <f>[3]f0_b0!F1</f>
-        <v>t.value</v>
+        <f>[1]utt_f0_b0!F1</f>
+        <v>z.value</v>
       </c>
       <c r="G2" s="8" t="str">
-        <f>[3]f0_b0!G1</f>
+        <f>[1]utt_f0_b0!G1</f>
         <v>df</v>
       </c>
       <c r="H2" s="8" t="str">
-        <f>[3]f0_b0!H1</f>
+        <f>[1]utt_f0_b0!H1</f>
         <v>p.value</v>
       </c>
       <c r="I2" s="9" t="str">
-        <f>[3]f0_b0!I1</f>
-        <v>p.adj. (bf=4)</v>
+        <f>[1]utt_f0_b0!I1</f>
+        <v>p.adj (BH)</v>
       </c>
       <c r="J2" s="9" t="str">
-        <f>[3]f0_b0!J1</f>
-        <v xml:space="preserve">signif. </v>
+        <f>[1]utt_f0_b0!J1</f>
+        <v>signif.</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>5</v>
@@ -3934,186 +4163,186 @@
     </row>
     <row r="3" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="str">
-        <f>RIGHT([3]f0_b0!A2,3)</f>
+        <f>RIGHT([1]utt_f0_b0!A2,3)</f>
         <v>MDC</v>
       </c>
       <c r="B3" s="12">
-        <f>[3]f0_b0!B2</f>
-        <v>86.081999999999994</v>
+        <f>[1]utt_f0_b0!B2</f>
+        <v>89.230999999999995</v>
       </c>
       <c r="C3" s="12">
-        <f>[3]f0_b0!C2</f>
-        <v>1.5149999999999999</v>
+        <f>[1]utt_f0_b0!C2</f>
+        <v>1.127</v>
       </c>
       <c r="D3" s="12">
-        <f>[3]f0_b0!D2</f>
-        <v>83.111999999999995</v>
+        <f>[1]utt_f0_b0!D2</f>
+        <v>87.022000000000006</v>
       </c>
       <c r="E3" s="12">
-        <f>[3]f0_b0!E2</f>
-        <v>89.052000000000007</v>
+        <f>[1]utt_f0_b0!E2</f>
+        <v>91.44</v>
       </c>
       <c r="F3" s="12">
-        <f>[3]f0_b0!F2</f>
-        <v>56.805</v>
+        <f>[1]utt_f0_b0!F2</f>
+        <v>79.168999999999997</v>
       </c>
       <c r="G3" s="12">
-        <f>[3]f0_b0!G2</f>
-        <v>10</v>
+        <f>[1]utt_f0_b0!G2</f>
+        <v>11.69</v>
       </c>
       <c r="H3" s="13">
-        <f>[3]f0_b0!H2</f>
-        <v>6.9199999999999998E-14</v>
+        <f>[1]utt_f0_b0!H2</f>
+        <v>2.5500000000000001E-17</v>
       </c>
       <c r="I3" s="13">
-        <f>[3]f0_b0!I2</f>
-        <v>2.7699999999999998E-13</v>
+        <f>[1]utt_f0_b0!I2</f>
+        <v>2.0400000000000001E-16</v>
       </c>
       <c r="J3" s="14" t="str">
-        <f>[3]f0_b0!J2</f>
-        <v>p&lt;0.001</v>
+        <f>[1]utt_f0_b0!J2</f>
+        <v>p&lt;0.0001</v>
       </c>
       <c r="K3" s="12">
         <f>B3-D3</f>
-        <v>2.9699999999999989</v>
+        <v>2.208999999999989</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="str">
-        <f>RIGHT([3]f0_b0!A3,3)</f>
+        <f>RIGHT([1]utt_f0_b0!A3,3)</f>
         <v>MWH</v>
       </c>
       <c r="B4" s="17">
-        <f>[3]f0_b0!B3</f>
-        <v>86.551000000000002</v>
+        <f>[1]utt_f0_b0!B3</f>
+        <v>89.652000000000001</v>
       </c>
       <c r="C4" s="17">
-        <f>[3]f0_b0!C3</f>
-        <v>1.3520000000000001</v>
+        <f>[1]utt_f0_b0!C3</f>
+        <v>0.98099999999999998</v>
       </c>
       <c r="D4" s="17">
-        <f>[3]f0_b0!D3</f>
-        <v>83.900999999999996</v>
+        <f>[1]utt_f0_b0!D3</f>
+        <v>87.73</v>
       </c>
       <c r="E4" s="17">
-        <f>[3]f0_b0!E3</f>
-        <v>89.200999999999993</v>
+        <f>[1]utt_f0_b0!E3</f>
+        <v>91.573999999999998</v>
       </c>
       <c r="F4" s="17">
-        <f>[3]f0_b0!F3</f>
-        <v>64.013000000000005</v>
+        <f>[1]utt_f0_b0!F3</f>
+        <v>91.424999999999997</v>
       </c>
       <c r="G4" s="17">
-        <f>[3]f0_b0!G3</f>
-        <v>10</v>
+        <f>[1]utt_f0_b0!G3</f>
+        <v>10.119999999999999</v>
       </c>
       <c r="H4" s="18">
-        <f>[3]f0_b0!H3</f>
-        <v>2.1027E-14</v>
+        <f>[1]utt_f0_b0!H3</f>
+        <v>4.28E-16</v>
       </c>
       <c r="I4" s="18">
-        <f>[3]f0_b0!I3</f>
-        <v>8.4100000000000003E-14</v>
+        <f>[1]utt_f0_b0!I3</f>
+        <v>2.57E-15</v>
       </c>
       <c r="J4" s="19" t="str">
-        <f>[3]f0_b0!J3</f>
-        <v>p&lt;0.001</v>
+        <f>[1]utt_f0_b0!J3</f>
+        <v>p&lt;0.0001</v>
       </c>
       <c r="K4" s="17">
         <f t="shared" ref="K4:K6" si="0">B4-D4</f>
-        <v>2.6500000000000057</v>
+        <v>1.921999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="str">
-        <f>RIGHT([3]f0_b0!A4,3)</f>
+        <f>RIGHT([1]utt_f0_b0!A4,3)</f>
         <v>MYN</v>
       </c>
       <c r="B5" s="17">
-        <f>[3]f0_b0!B4</f>
-        <v>86.840999999999994</v>
+        <f>[1]utt_f0_b0!B4</f>
+        <v>90.016999999999996</v>
       </c>
       <c r="C5" s="17">
-        <f>[3]f0_b0!C4</f>
-        <v>1.387</v>
+        <f>[1]utt_f0_b0!C4</f>
+        <v>1.0660000000000001</v>
       </c>
       <c r="D5" s="17">
-        <f>[3]f0_b0!D4</f>
-        <v>84.123000000000005</v>
+        <f>[1]utt_f0_b0!D4</f>
+        <v>87.927999999999997</v>
       </c>
       <c r="E5" s="17">
-        <f>[3]f0_b0!E4</f>
-        <v>89.56</v>
+        <f>[1]utt_f0_b0!E4</f>
+        <v>92.106999999999999</v>
       </c>
       <c r="F5" s="17">
-        <f>[3]f0_b0!F4</f>
-        <v>62.616</v>
+        <f>[1]utt_f0_b0!F4</f>
+        <v>84.435000000000002</v>
       </c>
       <c r="G5" s="17">
-        <f>[3]f0_b0!G4</f>
-        <v>10</v>
+        <f>[1]utt_f0_b0!G4</f>
+        <v>11.53</v>
       </c>
       <c r="H5" s="18">
-        <f>[3]f0_b0!H4</f>
-        <v>2.6189E-14</v>
+        <f>[1]utt_f0_b0!H4</f>
+        <v>1.86E-17</v>
       </c>
       <c r="I5" s="18">
-        <f>[3]f0_b0!I4</f>
-        <v>1.0499999999999999E-13</v>
+        <f>[1]utt_f0_b0!I4</f>
+        <v>2.0400000000000001E-16</v>
       </c>
       <c r="J5" s="19" t="str">
-        <f>[3]f0_b0!J4</f>
-        <v>p&lt;0.001</v>
+        <f>[1]utt_f0_b0!J4</f>
+        <v>p&lt;0.0001</v>
       </c>
       <c r="K5" s="17">
         <f t="shared" si="0"/>
-        <v>2.7179999999999893</v>
+        <v>2.0889999999999986</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="str">
-        <f>RIGHT([3]f0_b0!A5,3)</f>
+        <f>RIGHT([1]utt_f0_b0!A5,3)</f>
         <v>MDQ</v>
       </c>
       <c r="B6" s="21">
-        <f>[3]f0_b0!B5</f>
-        <v>88.369</v>
+        <f>[1]utt_f0_b0!B5</f>
+        <v>91.546999999999997</v>
       </c>
       <c r="C6" s="21">
-        <f>[3]f0_b0!C5</f>
-        <v>1.591</v>
+        <f>[1]utt_f0_b0!C5</f>
+        <v>1.3160000000000001</v>
       </c>
       <c r="D6" s="21">
-        <f>[3]f0_b0!D5</f>
-        <v>85.251000000000005</v>
+        <f>[1]utt_f0_b0!D5</f>
+        <v>88.968000000000004</v>
       </c>
       <c r="E6" s="21">
-        <f>[3]f0_b0!E5</f>
-        <v>91.486999999999995</v>
+        <f>[1]utt_f0_b0!E5</f>
+        <v>94.126000000000005</v>
       </c>
       <c r="F6" s="21">
-        <f>[3]f0_b0!F5</f>
-        <v>55.555</v>
+        <f>[1]utt_f0_b0!F5</f>
+        <v>69.561999999999998</v>
       </c>
       <c r="G6" s="21">
-        <f>[3]f0_b0!G5</f>
-        <v>10</v>
+        <f>[1]utt_f0_b0!G5</f>
+        <v>12.73</v>
       </c>
       <c r="H6" s="22">
-        <f>[3]f0_b0!H5</f>
-        <v>8.6136E-14</v>
+        <f>[1]utt_f0_b0!H5</f>
+        <v>8.2800000000000006E-18</v>
       </c>
       <c r="I6" s="22">
-        <f>[3]f0_b0!I5</f>
-        <v>3.4499999999999999E-13</v>
+        <f>[1]utt_f0_b0!I5</f>
+        <v>1.99E-16</v>
       </c>
       <c r="J6" s="23" t="str">
-        <f>[3]f0_b0!J5</f>
-        <v>p&lt;0.001</v>
+        <f>[1]utt_f0_b0!J5</f>
+        <v>p&lt;0.0001</v>
       </c>
       <c r="K6" s="21">
         <f t="shared" si="0"/>
-        <v>3.117999999999995</v>
+        <v>2.5789999999999935</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -4136,51 +4365,54 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
+      <c r="G8" s="32" t="s">
+        <v>9</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" s="10" customFormat="1" ht="25.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>0</v>
+    <row r="9" spans="1:11" ht="25.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="str">
+        <f>[2]utt_slope_b0!A1</f>
+        <v>intercept</v>
       </c>
       <c r="B9" s="8" t="str">
-        <f>[1]slope_b0!B1</f>
+        <f>[2]utt_slope_b0!B1</f>
         <v>estimate</v>
       </c>
       <c r="C9" s="8" t="str">
-        <f>[1]slope_b0!C1</f>
+        <f>[2]utt_slope_b0!C1</f>
         <v>std.error</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>[1]slope_b0!D1</f>
+        <f>[2]utt_slope_b0!D1</f>
         <v>2.5% CI</v>
       </c>
       <c r="E9" s="8" t="str">
-        <f>[1]slope_b0!E1</f>
+        <f>[2]utt_slope_b0!E1</f>
         <v>97.5% CI</v>
       </c>
       <c r="F9" s="8" t="str">
-        <f>[1]slope_b0!F1</f>
-        <v>t.value</v>
+        <f>[2]utt_slope_b0!F1</f>
+        <v>z.value</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>[1]slope_b0!G1</f>
+        <f>[2]utt_slope_b0!G1</f>
         <v>df</v>
       </c>
       <c r="H9" s="8" t="str">
-        <f>[1]slope_b0!H1</f>
+        <f>[2]utt_slope_b0!H1</f>
         <v>p.value</v>
       </c>
       <c r="I9" s="9" t="str">
-        <f>[1]slope_b0!I1</f>
-        <v>p.adj. (bf=4)</v>
+        <f>[2]utt_slope_b0!I1</f>
+        <v>p.adj (BH)</v>
       </c>
       <c r="J9" s="9" t="str">
-        <f>[1]slope_b0!J1</f>
-        <v xml:space="preserve">signif. </v>
+        <f>[2]utt_slope_b0!J1</f>
+        <v>signif.</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>5</v>
@@ -4191,44 +4423,44 @@
         <v>0</v>
       </c>
       <c r="B10" s="12">
-        <f>[1]slope_b0!B2</f>
-        <v>-0.42</v>
+        <f>[2]utt_slope_b0!B2</f>
+        <v>-1.694</v>
       </c>
       <c r="C10" s="12">
-        <f>[1]slope_b0!C2</f>
-        <v>0.69899999999999995</v>
+        <f>[2]utt_slope_b0!C2</f>
+        <v>0.76500000000000001</v>
       </c>
       <c r="D10" s="12">
-        <f>[1]slope_b0!D2</f>
-        <v>-1.79</v>
+        <f>[2]utt_slope_b0!D2</f>
+        <v>-3.194</v>
       </c>
       <c r="E10" s="12">
-        <f>[1]slope_b0!E2</f>
-        <v>0.94899999999999995</v>
+        <f>[2]utt_slope_b0!E2</f>
+        <v>-0.19400000000000001</v>
       </c>
       <c r="F10" s="12">
-        <f>[1]slope_b0!F2</f>
-        <v>-0.60199999999999998</v>
+        <f>[2]utt_slope_b0!F2</f>
+        <v>-2.2130000000000001</v>
       </c>
       <c r="G10" s="12">
-        <f>[1]slope_b0!G2</f>
-        <v>9.9700000000000006</v>
+        <f>[2]utt_slope_b0!G2</f>
+        <v>13.41</v>
       </c>
       <c r="H10" s="13">
-        <f>[1]slope_b0!H2</f>
-        <v>0.56079999999999997</v>
+        <f>[2]utt_slope_b0!H2</f>
+        <v>4.48E-2</v>
       </c>
       <c r="I10" s="13">
-        <f>[1]slope_b0!I2</f>
-        <v>0.99990000000000001</v>
+        <f>[2]utt_slope_b0!I2</f>
+        <v>5.3800000000000001E-2</v>
       </c>
       <c r="J10" s="14">
-        <f>[1]slope_b0!J2</f>
+        <f>[2]utt_slope_b0!J2</f>
         <v>0</v>
       </c>
       <c r="K10" s="12">
         <f>B10-D10</f>
-        <v>1.37</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4236,44 +4468,44 @@
         <v>1</v>
       </c>
       <c r="B11" s="17">
-        <f>[1]slope_b0!B3</f>
-        <v>-2.8439999999999999</v>
+        <f>[2]utt_slope_b0!B3</f>
+        <v>-3.7210000000000001</v>
       </c>
       <c r="C11" s="17">
-        <f>[1]slope_b0!C3</f>
-        <v>0.875</v>
+        <f>[2]utt_slope_b0!C3</f>
+        <v>1.0780000000000001</v>
       </c>
       <c r="D11" s="17">
-        <f>[1]slope_b0!D3</f>
-        <v>-4.5590000000000002</v>
+        <f>[2]utt_slope_b0!D3</f>
+        <v>-5.835</v>
       </c>
       <c r="E11" s="17">
-        <f>[1]slope_b0!E3</f>
-        <v>-1.129</v>
+        <f>[2]utt_slope_b0!E3</f>
+        <v>-1.6080000000000001</v>
       </c>
       <c r="F11" s="17">
-        <f>[1]slope_b0!F3</f>
-        <v>-3.25</v>
+        <f>[2]utt_slope_b0!F3</f>
+        <v>-3.4510000000000001</v>
       </c>
       <c r="G11" s="17">
-        <f>[1]slope_b0!G3</f>
-        <v>9.99</v>
+        <f>[2]utt_slope_b0!G3</f>
+        <v>9.61</v>
       </c>
       <c r="H11" s="18">
-        <f>[1]slope_b0!H3</f>
-        <v>8.6999999999999994E-3</v>
+        <f>[2]utt_slope_b0!H3</f>
+        <v>6.6E-3</v>
       </c>
       <c r="I11" s="18">
-        <f>[1]slope_b0!I3</f>
-        <v>3.49E-2</v>
+        <f>[2]utt_slope_b0!I3</f>
+        <v>1.18E-2</v>
       </c>
       <c r="J11" s="19" t="str">
-        <f>[1]slope_b0!J3</f>
+        <f>[2]utt_slope_b0!J3</f>
         <v>p&lt;0.05</v>
       </c>
       <c r="K11" s="17">
         <f t="shared" ref="K11:K13" si="1">B11-D11</f>
-        <v>1.7150000000000003</v>
+        <v>2.1139999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4281,44 +4513,44 @@
         <v>2</v>
       </c>
       <c r="B12" s="17">
-        <f>[1]slope_b0!B4</f>
-        <v>3.12</v>
+        <f>[2]utt_slope_b0!B4</f>
+        <v>1.7</v>
       </c>
       <c r="C12" s="17">
-        <f>[1]slope_b0!C4</f>
-        <v>0.66200000000000003</v>
+        <f>[2]utt_slope_b0!C4</f>
+        <v>0.627</v>
       </c>
       <c r="D12" s="17">
-        <f>[1]slope_b0!D4</f>
-        <v>1.8220000000000001</v>
+        <f>[2]utt_slope_b0!D4</f>
+        <v>0.47199999999999998</v>
       </c>
       <c r="E12" s="17">
-        <f>[1]slope_b0!E4</f>
-        <v>4.4169999999999998</v>
+        <f>[2]utt_slope_b0!E4</f>
+        <v>2.9289999999999998</v>
       </c>
       <c r="F12" s="17">
-        <f>[1]slope_b0!F4</f>
-        <v>4.7130000000000001</v>
+        <f>[2]utt_slope_b0!F4</f>
+        <v>2.7130000000000001</v>
       </c>
       <c r="G12" s="17">
-        <f>[1]slope_b0!G4</f>
-        <v>10.029999999999999</v>
+        <f>[2]utt_slope_b0!G4</f>
+        <v>10.58</v>
       </c>
       <c r="H12" s="18">
-        <f>[1]slope_b0!H4</f>
-        <v>8.1840999999999999E-4</v>
+        <f>[2]utt_slope_b0!H4</f>
+        <v>2.0799999999999999E-2</v>
       </c>
       <c r="I12" s="18">
-        <f>[1]slope_b0!I4</f>
-        <v>3.3E-3</v>
+        <f>[2]utt_slope_b0!I4</f>
+        <v>2.7799999999999998E-2</v>
       </c>
       <c r="J12" s="19" t="str">
-        <f>[1]slope_b0!J4</f>
-        <v>p&lt;0.01</v>
+        <f>[2]utt_slope_b0!J4</f>
+        <v>p&lt;0.05</v>
       </c>
       <c r="K12" s="17">
         <f t="shared" si="1"/>
-        <v>1.298</v>
+        <v>1.228</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4326,351 +4558,236 @@
         <v>3</v>
       </c>
       <c r="B13" s="21">
-        <f>[1]slope_b0!B5</f>
-        <v>6.0960000000000001</v>
+        <f>[2]utt_slope_b0!B5</f>
+        <v>4.6859999999999999</v>
       </c>
       <c r="C13" s="21">
-        <f>[1]slope_b0!C5</f>
-        <v>1.0489999999999999</v>
+        <f>[2]utt_slope_b0!C5</f>
+        <v>1.129</v>
       </c>
       <c r="D13" s="21">
-        <f>[1]slope_b0!D5</f>
-        <v>4.0389999999999997</v>
+        <f>[2]utt_slope_b0!D5</f>
+        <v>2.472</v>
       </c>
       <c r="E13" s="21">
-        <f>[1]slope_b0!E5</f>
-        <v>8.1530000000000005</v>
+        <f>[2]utt_slope_b0!E5</f>
+        <v>6.899</v>
       </c>
       <c r="F13" s="21">
-        <f>[1]slope_b0!F5</f>
-        <v>5.8090000000000002</v>
+        <f>[2]utt_slope_b0!F5</f>
+        <v>4.149</v>
       </c>
       <c r="G13" s="21">
-        <f>[1]slope_b0!G5</f>
-        <v>10.039999999999999</v>
+        <f>[2]utt_slope_b0!G5</f>
+        <v>12.74</v>
       </c>
       <c r="H13" s="22">
-        <f>[1]slope_b0!H5</f>
-        <v>1.6829E-4</v>
+        <f>[2]utt_slope_b0!H5</f>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="I13" s="22">
-        <f>[1]slope_b0!I5</f>
-        <v>6.7299999999999999E-4</v>
+        <f>[2]utt_slope_b0!I5</f>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="J13" s="23" t="str">
-        <f>[1]slope_b0!J5</f>
-        <v>p&lt;0.001</v>
+        <f>[2]utt_slope_b0!J5</f>
+        <v>p&lt;0.01</v>
       </c>
       <c r="K13" s="21">
         <f t="shared" si="1"/>
-        <v>2.0570000000000004</v>
+        <v>2.214</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="33"/>
       <c r="G14" s="33"/>
-      <c r="K14" s="34"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-    </row>
-    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-    </row>
-    <row r="17" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-    </row>
-    <row r="18" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-    </row>
-    <row r="19" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-    </row>
-    <row r="20" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-    </row>
-    <row r="22" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="34"/>
-      <c r="K22" s="34"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="34"/>
-      <c r="K23" s="34"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
     </row>
-    <row r="24" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
-      <c r="B24" s="35"/>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="34"/>
-      <c r="K24" s="34"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
     </row>
-    <row r="25" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
-      <c r="B25" s="35"/>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C25" s="34"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="34"/>
-      <c r="K25" s="34"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
-      <c r="B26" s="35"/>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C26" s="34"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="34"/>
-      <c r="K26" s="34"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
     </row>
-    <row r="28" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
-      <c r="B28" s="35"/>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C28" s="34"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="34"/>
-      <c r="K28" s="34"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
-      <c r="B29" s="35"/>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C29" s="34"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="34"/>
-      <c r="K29" s="34"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
     </row>
-    <row r="30" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
-      <c r="B30" s="35"/>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C30" s="34"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="34"/>
-      <c r="K30" s="34"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
     </row>
-    <row r="31" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
-      <c r="B31" s="35"/>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C31" s="34"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="34"/>
-      <c r="K31" s="34"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
     </row>
-    <row r="32" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
-      <c r="B32" s="35"/>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C32" s="34"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="34"/>
-      <c r="K32" s="34"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="H10:I11">
-    <cfRule type="cellIs" dxfId="77" priority="53" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="55" stopIfTrue="1" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="54" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="56" stopIfTrue="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="55" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="57" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="56" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="58" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:J11">
-    <cfRule type="containsText" dxfId="73" priority="49" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
+    <cfRule type="containsText" dxfId="62" priority="51" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.001",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="50" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
+    <cfRule type="containsText" dxfId="61" priority="52" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.01",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="51" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
+    <cfRule type="containsText" dxfId="60" priority="53" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.05",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="52" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
+    <cfRule type="containsText" dxfId="59" priority="54" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.1",J10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:I13">
-    <cfRule type="cellIs" dxfId="69" priority="45" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="47" stopIfTrue="1" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="46" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="48" stopIfTrue="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="47" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="49" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="48" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="50" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J13">
-    <cfRule type="containsText" dxfId="65" priority="41" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
+    <cfRule type="containsText" dxfId="54" priority="43" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.001",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="42" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
+    <cfRule type="containsText" dxfId="53" priority="44" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.01",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="43" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
+    <cfRule type="containsText" dxfId="52" priority="45" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.05",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="44" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
+    <cfRule type="containsText" dxfId="51" priority="46" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.1",J12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I4">
-    <cfRule type="cellIs" dxfId="29" priority="13" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="15" stopIfTrue="1" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="15" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="17" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="16" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="18" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J4">
-    <cfRule type="containsText" dxfId="25" priority="9" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
+    <cfRule type="containsText" dxfId="46" priority="11" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.001",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="10" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
+    <cfRule type="containsText" dxfId="45" priority="12" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.01",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="11" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
+    <cfRule type="containsText" dxfId="44" priority="13" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.05",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="12" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
+    <cfRule type="containsText" dxfId="43" priority="14" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.1",J3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="2" stopIfTrue="1" operator="containsText" text="p&lt;0.0001">
+      <formula>NOT(ISERROR(SEARCH("p&lt;0.0001",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:I6">
-    <cfRule type="cellIs" dxfId="21" priority="5" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="8" stopIfTrue="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="9" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J6">
-    <cfRule type="containsText" dxfId="17" priority="1" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
+    <cfRule type="containsText" dxfId="37" priority="3" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.001",J5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
+    <cfRule type="containsText" dxfId="36" priority="4" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.01",J5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="3" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
+    <cfRule type="containsText" dxfId="35" priority="5" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.05",J5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="4" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
+    <cfRule type="containsText" dxfId="34" priority="6" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.1",J5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="1" stopIfTrue="1" operator="containsText" text="p&lt;0.0001">
+      <formula>NOT(ISERROR(SEARCH("p&lt;0.0001",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4707,48 +4824,48 @@
     </row>
     <row r="2" spans="1:14" ht="25.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="str">
-        <f>RIGHT([4]f0_b1!A1,3)</f>
-        <v>ept</v>
+        <f>[3]utt_f0_b1!A1</f>
+        <v>intercept</v>
       </c>
       <c r="B2" s="8" t="str">
-        <f>RIGHT([4]f0_b1!B1,3)</f>
-        <v>ope</v>
+        <f>[3]utt_f0_b1!B1</f>
+        <v>slope</v>
       </c>
       <c r="C2" s="8" t="str">
-        <f>[4]f0_b1!C1</f>
+        <f>[3]utt_f0_b1!C1</f>
         <v>estimate</v>
       </c>
       <c r="D2" s="8" t="str">
-        <f>[4]f0_b1!D1</f>
+        <f>[3]utt_f0_b1!D1</f>
         <v>std.error</v>
       </c>
       <c r="E2" s="8" t="str">
-        <f>[4]f0_b1!E1</f>
+        <f>[3]utt_f0_b1!E1</f>
         <v>2.5% CI</v>
       </c>
       <c r="F2" s="8" t="str">
-        <f>[4]f0_b1!F1</f>
+        <f>[3]utt_f0_b1!F1</f>
         <v>97.5% CI</v>
       </c>
       <c r="G2" s="8" t="str">
-        <f>[4]f0_b1!G1</f>
-        <v>t.value</v>
+        <f>[3]utt_f0_b1!G1</f>
+        <v>z.value</v>
       </c>
       <c r="H2" s="8" t="str">
-        <f>[4]f0_b1!H1</f>
+        <f>[3]utt_f0_b1!H1</f>
         <v>df</v>
       </c>
       <c r="I2" s="9" t="str">
-        <f>[4]f0_b1!I1</f>
+        <f>[3]utt_f0_b1!I1</f>
         <v>p.value</v>
       </c>
       <c r="J2" s="9" t="str">
-        <f>[4]f0_b1!J1</f>
-        <v>p.adj. (bf=4)</v>
+        <f>[3]utt_f0_b1!J1</f>
+        <v>p.adj (BH)</v>
       </c>
       <c r="K2" s="8" t="str">
-        <f>[4]f0_b1!K1</f>
-        <v xml:space="preserve">signif. </v>
+        <f>[3]utt_f0_b1!K1</f>
+        <v>signif.</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>7</v>
@@ -4759,286 +4876,286 @@
     </row>
     <row r="3" spans="1:14" ht="33.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="str">
-        <f>RIGHT([4]f0_b1!A2,3)</f>
+        <f>RIGHT([3]utt_f0_b1!A2,3)</f>
         <v>MDC</v>
       </c>
       <c r="B3" s="12" t="str">
-        <f>RIGHT([4]f0_b1!B2,3)</f>
+        <f>RIGHT([3]utt_f0_b1!B2,3)</f>
         <v>MWH</v>
       </c>
       <c r="C3" s="12">
-        <f>[4]f0_b1!C2</f>
-        <v>0.47</v>
+        <f>[3]utt_f0_b1!C2</f>
+        <v>0.42099999999999999</v>
       </c>
       <c r="D3" s="12">
-        <f>[4]f0_b1!D2</f>
-        <v>0.311</v>
+        <f>[3]utt_f0_b1!D2</f>
+        <v>0.312</v>
       </c>
       <c r="E3" s="12">
-        <f>[4]f0_b1!E2</f>
-        <v>-0.13900000000000001</v>
+        <f>[3]utt_f0_b1!E2</f>
+        <v>-0.191</v>
       </c>
       <c r="F3" s="12">
-        <f>[4]f0_b1!F2</f>
-        <v>1.0780000000000001</v>
+        <f>[3]utt_f0_b1!F2</f>
+        <v>1.0329999999999999</v>
       </c>
       <c r="G3" s="12">
-        <f>[4]f0_b1!G2</f>
-        <v>1.5129999999999999</v>
+        <f>[3]utt_f0_b1!G2</f>
+        <v>1.349</v>
       </c>
       <c r="H3" s="13">
-        <f>[4]f0_b1!H2</f>
-        <v>10.07</v>
+        <f>[3]utt_f0_b1!H2</f>
+        <v>10.8</v>
       </c>
       <c r="I3" s="13">
-        <f>[4]f0_b1!I2</f>
-        <v>0.16109999999999999</v>
+        <f>[3]utt_f0_b1!I2</f>
+        <v>0.2051</v>
       </c>
       <c r="J3" s="38">
-        <f>[4]f0_b1!J2</f>
-        <v>0.64439999999999997</v>
+        <f>[3]utt_f0_b1!J2</f>
+        <v>0.214</v>
       </c>
       <c r="K3" s="11">
-        <f>[4]f0_b1!K2</f>
+        <f>[3]utt_f0_b1!K2</f>
         <v>0</v>
       </c>
       <c r="M3" s="39">
-        <f>[5]f0_r2!$B$3</f>
-        <v>2.8174816408763698E-2</v>
+        <f>[4]utt_f0_r2!$B$3</f>
+        <v>0.52849012129538697</v>
       </c>
       <c r="N3" s="39">
-        <f>[5]f0_r2!$B$2</f>
-        <v>0.94762073814392001</v>
+        <f>[4]utt_f0_r2!$B$2</f>
+        <v>0.94231623989217705</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="str">
-        <f>RIGHT([4]f0_b1!A3,3)</f>
+        <f>RIGHT([3]utt_f0_b1!A3,3)</f>
         <v>MDC</v>
       </c>
       <c r="B4" s="17" t="str">
-        <f>RIGHT([4]f0_b1!B3,3)</f>
+        <f>RIGHT([3]utt_f0_b1!B3,3)</f>
         <v>MYN</v>
       </c>
       <c r="C4" s="17">
-        <f>[4]f0_b1!C3</f>
-        <v>0.76</v>
+        <f>[3]utt_f0_b1!C3</f>
+        <v>0.78600000000000003</v>
       </c>
       <c r="D4" s="17">
-        <f>[4]f0_b1!D3</f>
-        <v>0.249</v>
+        <f>[3]utt_f0_b1!D3</f>
+        <v>0.25</v>
       </c>
       <c r="E4" s="17">
-        <f>[4]f0_b1!E3</f>
-        <v>0.27200000000000002</v>
+        <f>[3]utt_f0_b1!E3</f>
+        <v>0.29599999999999999</v>
       </c>
       <c r="F4" s="17">
-        <f>[4]f0_b1!F3</f>
-        <v>1.2470000000000001</v>
+        <f>[3]utt_f0_b1!F3</f>
+        <v>1.2769999999999999</v>
       </c>
       <c r="G4" s="17">
-        <f>[4]f0_b1!G3</f>
-        <v>3.0510000000000002</v>
+        <f>[3]utt_f0_b1!G3</f>
+        <v>3.1419999999999999</v>
       </c>
       <c r="H4" s="18">
-        <f>[4]f0_b1!H3</f>
-        <v>10.07</v>
+        <f>[3]utt_f0_b1!H3</f>
+        <v>10.37</v>
       </c>
       <c r="I4" s="18">
-        <f>[4]f0_b1!I3</f>
-        <v>1.21E-2</v>
+        <f>[3]utt_f0_b1!I3</f>
+        <v>0.01</v>
       </c>
       <c r="J4" s="40">
-        <f>[4]f0_b1!J3</f>
-        <v>4.8500000000000001E-2</v>
+        <f>[3]utt_f0_b1!J3</f>
+        <v>1.5100000000000001E-2</v>
       </c>
       <c r="K4" s="16" t="str">
-        <f>[4]f0_b1!K3</f>
+        <f>[3]utt_f0_b1!K3</f>
         <v>p&lt;0.05</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="str">
-        <f>RIGHT([4]f0_b1!A4,3)</f>
+        <f>RIGHT([3]utt_f0_b1!A4,3)</f>
         <v>MDC</v>
       </c>
       <c r="B5" s="17" t="str">
-        <f>RIGHT([4]f0_b1!B4,3)</f>
+        <f>RIGHT([3]utt_f0_b1!B4,3)</f>
         <v>MDQ</v>
       </c>
       <c r="C5" s="17">
-        <f>[4]f0_b1!C4</f>
-        <v>2.2869999999999999</v>
+        <f>[3]utt_f0_b1!C4</f>
+        <v>2.3159999999999998</v>
       </c>
       <c r="D5" s="17">
-        <f>[4]f0_b1!D4</f>
-        <v>0.438</v>
+        <f>[3]utt_f0_b1!D4</f>
+        <v>0.442</v>
       </c>
       <c r="E5" s="17">
-        <f>[4]f0_b1!E4</f>
-        <v>1.4279999999999999</v>
+        <f>[3]utt_f0_b1!E4</f>
+        <v>1.4490000000000001</v>
       </c>
       <c r="F5" s="17">
-        <f>[4]f0_b1!F4</f>
-        <v>3.1469999999999998</v>
+        <f>[3]utt_f0_b1!F4</f>
+        <v>3.1829999999999998</v>
       </c>
       <c r="G5" s="17">
-        <f>[4]f0_b1!G4</f>
-        <v>5.2160000000000002</v>
+        <f>[3]utt_f0_b1!G4</f>
+        <v>5.2370000000000001</v>
       </c>
       <c r="H5" s="18">
-        <f>[4]f0_b1!H4</f>
-        <v>10.06</v>
+        <f>[3]utt_f0_b1!H4</f>
+        <v>10.17</v>
       </c>
       <c r="I5" s="18">
-        <f>[4]f0_b1!I4</f>
-        <v>3.8405999999999998E-4</v>
+        <f>[3]utt_f0_b1!I4</f>
+        <v>3.6000000000000002E-4</v>
       </c>
       <c r="J5" s="40">
-        <f>[4]f0_b1!J4</f>
-        <v>1.5E-3</v>
+        <f>[3]utt_f0_b1!J4</f>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="K5" s="16" t="str">
-        <f>[4]f0_b1!K4</f>
+        <f>[3]utt_f0_b1!K4</f>
         <v>p&lt;0.01</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="str">
-        <f>RIGHT([4]f0_b1!A5,3)</f>
+        <f>RIGHT([3]utt_f0_b1!A5,3)</f>
         <v>MWH</v>
       </c>
       <c r="B6" s="17" t="str">
-        <f>RIGHT([4]f0_b1!B5,3)</f>
+        <f>RIGHT([3]utt_f0_b1!B5,3)</f>
         <v>MYN</v>
       </c>
       <c r="C6" s="17">
-        <f>[4]f0_b1!C5</f>
-        <v>0.28999999999999998</v>
+        <f>[3]utt_f0_b1!C5</f>
+        <v>0.36499999999999999</v>
       </c>
       <c r="D6" s="17">
-        <f>[4]f0_b1!D5</f>
-        <v>0.252</v>
+        <f>[3]utt_f0_b1!D5</f>
+        <v>0.26700000000000002</v>
       </c>
       <c r="E6" s="17">
-        <f>[4]f0_b1!E5</f>
-        <v>-0.20499999999999999</v>
+        <f>[3]utt_f0_b1!E5</f>
+        <v>-0.158</v>
       </c>
       <c r="F6" s="17">
-        <f>[4]f0_b1!F5</f>
-        <v>0.78500000000000003</v>
+        <f>[3]utt_f0_b1!F5</f>
+        <v>0.88900000000000001</v>
       </c>
       <c r="G6" s="17">
-        <f>[4]f0_b1!G5</f>
-        <v>1.1479999999999999</v>
+        <f>[3]utt_f0_b1!G5</f>
+        <v>1.3680000000000001</v>
       </c>
       <c r="H6" s="18">
-        <f>[4]f0_b1!H5</f>
-        <v>9.98</v>
+        <f>[3]utt_f0_b1!H5</f>
+        <v>12.73</v>
       </c>
       <c r="I6" s="18">
-        <f>[4]f0_b1!I5</f>
-        <v>0.27760000000000001</v>
+        <f>[3]utt_f0_b1!I5</f>
+        <v>0.1951</v>
       </c>
       <c r="J6" s="40">
-        <f>[4]f0_b1!J5</f>
-        <v>0.99990000000000001</v>
+        <f>[3]utt_f0_b1!J5</f>
+        <v>0.21290000000000001</v>
       </c>
       <c r="K6" s="16">
-        <f>[4]f0_b1!K5</f>
+        <f>[3]utt_f0_b1!K5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="str">
-        <f>RIGHT([4]f0_b1!A6,3)</f>
+        <f>RIGHT([3]utt_f0_b1!A6,3)</f>
         <v>MWH</v>
       </c>
       <c r="B7" s="17" t="str">
-        <f>RIGHT([4]f0_b1!B6,3)</f>
+        <f>RIGHT([3]utt_f0_b1!B6,3)</f>
         <v>MDQ</v>
       </c>
       <c r="C7" s="17">
-        <f>[4]f0_b1!C6</f>
-        <v>1.8169999999999999</v>
+        <f>[3]utt_f0_b1!C6</f>
+        <v>1.8959999999999999</v>
       </c>
       <c r="D7" s="17">
-        <f>[4]f0_b1!D6</f>
-        <v>0.63200000000000001</v>
+        <f>[3]utt_f0_b1!D6</f>
+        <v>0.63900000000000001</v>
       </c>
       <c r="E7" s="17">
-        <f>[4]f0_b1!E6</f>
-        <v>0.57999999999999996</v>
+        <f>[3]utt_f0_b1!E6</f>
+        <v>0.64400000000000002</v>
       </c>
       <c r="F7" s="17">
-        <f>[4]f0_b1!F6</f>
-        <v>3.0550000000000002</v>
+        <f>[3]utt_f0_b1!F6</f>
+        <v>3.1469999999999998</v>
       </c>
       <c r="G7" s="17">
-        <f>[4]f0_b1!G6</f>
-        <v>2.8780000000000001</v>
+        <f>[3]utt_f0_b1!G6</f>
+        <v>2.968</v>
       </c>
       <c r="H7" s="18">
-        <f>[4]f0_b1!H6</f>
-        <v>10.039999999999999</v>
+        <f>[3]utt_f0_b1!H6</f>
+        <v>10.51</v>
       </c>
       <c r="I7" s="18">
-        <f>[4]f0_b1!I6</f>
-        <v>1.6400000000000001E-2</v>
+        <f>[3]utt_f0_b1!I6</f>
+        <v>1.34E-2</v>
       </c>
       <c r="J7" s="40">
-        <f>[4]f0_b1!J6</f>
-        <v>6.5600000000000006E-2</v>
+        <f>[3]utt_f0_b1!J6</f>
+        <v>1.89E-2</v>
       </c>
       <c r="K7" s="16" t="str">
-        <f>[4]f0_b1!K6</f>
-        <v>(p&lt;0.1)</v>
+        <f>[3]utt_f0_b1!K6</f>
+        <v>p&lt;0.05</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="41" t="str">
-        <f>RIGHT([4]f0_b1!A7,3)</f>
+        <f>RIGHT([3]utt_f0_b1!A7,3)</f>
         <v>MYN</v>
       </c>
       <c r="B8" s="42" t="str">
-        <f>RIGHT([4]f0_b1!B7,3)</f>
+        <f>RIGHT([3]utt_f0_b1!B7,3)</f>
         <v>MDQ</v>
       </c>
       <c r="C8" s="42">
-        <f>[4]f0_b1!C7</f>
-        <v>1.528</v>
+        <f>[3]utt_f0_b1!C7</f>
+        <v>1.53</v>
       </c>
       <c r="D8" s="42">
-        <f>[4]f0_b1!D7</f>
-        <v>0.59099999999999997</v>
+        <f>[3]utt_f0_b1!D7</f>
+        <v>0.58799999999999997</v>
       </c>
       <c r="E8" s="42">
-        <f>[4]f0_b1!E7</f>
-        <v>0.37</v>
+        <f>[3]utt_f0_b1!E7</f>
+        <v>0.377</v>
       </c>
       <c r="F8" s="42">
-        <f>[4]f0_b1!F7</f>
-        <v>2.6859999999999999</v>
+        <f>[3]utt_f0_b1!F7</f>
+        <v>2.6829999999999998</v>
       </c>
       <c r="G8" s="42">
-        <f>[4]f0_b1!G7</f>
-        <v>2.585</v>
+        <f>[3]utt_f0_b1!G7</f>
+        <v>2.6019999999999999</v>
       </c>
       <c r="H8" s="43">
-        <f>[4]f0_b1!H7</f>
-        <v>10.06</v>
+        <f>[3]utt_f0_b1!H7</f>
+        <v>10.050000000000001</v>
       </c>
       <c r="I8" s="43">
-        <f>[4]f0_b1!I7</f>
-        <v>2.7099999999999999E-2</v>
+        <f>[3]utt_f0_b1!I7</f>
+        <v>2.63E-2</v>
       </c>
       <c r="J8" s="44">
-        <f>[4]f0_b1!J7</f>
-        <v>0.1082</v>
-      </c>
-      <c r="K8" s="41">
-        <f>[4]f0_b1!K7</f>
-        <v>0</v>
+        <f>[3]utt_f0_b1!J7</f>
+        <v>3.32E-2</v>
+      </c>
+      <c r="K8" s="41" t="str">
+        <f>[3]utt_f0_b1!K7</f>
+        <v>p&lt;0.05</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5048,48 +5165,48 @@
     </row>
     <row r="11" spans="1:14" ht="25.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="str">
-        <f>[2]slope_b1!A1</f>
+        <f>[6]utt_slope_b1!A1</f>
         <v>intercept</v>
       </c>
       <c r="B11" s="8" t="str">
-        <f>[2]slope_b1!B1</f>
+        <f>[6]utt_slope_b1!B1</f>
         <v>slope</v>
       </c>
       <c r="C11" s="8" t="str">
-        <f>[2]slope_b1!C1</f>
+        <f>[6]utt_slope_b1!C1</f>
         <v>estimate</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f>[2]slope_b1!D1</f>
+        <f>[6]utt_slope_b1!D1</f>
         <v>std.error</v>
       </c>
       <c r="E11" s="8" t="str">
-        <f>[2]slope_b1!E1</f>
+        <f>[6]utt_slope_b1!E1</f>
         <v>2.5% CI</v>
       </c>
       <c r="F11" s="8" t="str">
-        <f>[2]slope_b1!F1</f>
+        <f>[6]utt_slope_b1!F1</f>
         <v>97.5% CI</v>
       </c>
       <c r="G11" s="8" t="str">
-        <f>[2]slope_b1!G1</f>
-        <v>t.value</v>
+        <f>[6]utt_slope_b1!G1</f>
+        <v>z.value</v>
       </c>
       <c r="H11" s="8" t="str">
-        <f>[2]slope_b1!H1</f>
+        <f>[6]utt_slope_b1!H1</f>
         <v>df</v>
       </c>
       <c r="I11" s="9" t="str">
-        <f>[2]slope_b1!I1</f>
+        <f>[6]utt_slope_b1!I1</f>
         <v>p.value</v>
       </c>
       <c r="J11" s="9" t="str">
-        <f>[2]slope_b1!J1</f>
-        <v>p.adj. (bf=4)</v>
+        <f>[6]utt_slope_b1!J1</f>
+        <v>p.adj (BH)</v>
       </c>
       <c r="K11" s="8" t="str">
-        <f>[2]slope_b1!K1</f>
-        <v xml:space="preserve">signif. </v>
+        <f>[6]utt_slope_b1!K1</f>
+        <v>signif.</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>7</v>
@@ -5100,338 +5217,338 @@
     </row>
     <row r="12" spans="1:14" ht="33.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="str">
-        <f>RIGHT([2]slope_b1!A2,3)</f>
+        <f>RIGHT([6]utt_slope_b1!A2,3)</f>
         <v>MDC</v>
       </c>
       <c r="B12" s="12" t="str">
-        <f>RIGHT([2]slope_b1!B2,3)</f>
+        <f>RIGHT([6]utt_slope_b1!B2,3)</f>
         <v>MWH</v>
       </c>
       <c r="C12" s="12">
-        <f>[2]slope_b1!C2</f>
-        <v>-2.423</v>
+        <f>[6]utt_slope_b1!C2</f>
+        <v>-2.028</v>
       </c>
       <c r="D12" s="12">
-        <f>[2]slope_b1!D2</f>
-        <v>1.2310000000000001</v>
+        <f>[6]utt_slope_b1!D2</f>
+        <v>1.234</v>
       </c>
       <c r="E12" s="12">
-        <f>[2]slope_b1!E2</f>
-        <v>-4.835</v>
+        <f>[6]utt_slope_b1!E2</f>
+        <v>-4.4470000000000001</v>
       </c>
       <c r="F12" s="12">
-        <f>[2]slope_b1!F2</f>
-        <v>-1.2E-2</v>
+        <f>[6]utt_slope_b1!F2</f>
+        <v>0.39200000000000002</v>
       </c>
       <c r="G12" s="12">
-        <f>[2]slope_b1!G2</f>
-        <v>-1.9690000000000001</v>
+        <f>[6]utt_slope_b1!G2</f>
+        <v>-1.643</v>
       </c>
       <c r="H12" s="12">
-        <f>[2]slope_b1!H2</f>
-        <v>9.99</v>
+        <f>[6]utt_slope_b1!H2</f>
+        <v>10.15</v>
       </c>
       <c r="I12" s="13">
-        <f>[2]slope_b1!I2</f>
-        <v>7.7200000000000005E-2</v>
+        <f>[6]utt_slope_b1!I2</f>
+        <v>0.13100000000000001</v>
       </c>
       <c r="J12" s="14">
-        <f>[2]slope_b1!J2</f>
-        <v>0.30890000000000001</v>
+        <f>[6]utt_slope_b1!J2</f>
+        <v>0.14979999999999999</v>
       </c>
       <c r="K12" s="11">
-        <f>[2]slope_b1!K2</f>
+        <f>[6]utt_slope_b1!K2</f>
         <v>0</v>
       </c>
       <c r="M12" s="39">
-        <f>[6]slope_r2!$B$3</f>
-        <v>0.48829263568562897</v>
+        <f>[5]utt_slope_r2!$B$3</f>
+        <v>0.51029969546325904</v>
       </c>
       <c r="N12" s="39">
-        <f>[6]slope_r2!$B$2</f>
-        <v>0.80018328350564605</v>
+        <f>[5]utt_slope_r2!$B$2</f>
+        <v>0.83641134398527495</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="str">
-        <f>RIGHT([2]slope_b1!A3,3)</f>
+        <f>RIGHT([6]utt_slope_b1!A3,3)</f>
         <v>MDC</v>
       </c>
       <c r="B13" s="17" t="str">
-        <f>RIGHT([2]slope_b1!B3,3)</f>
+        <f>RIGHT([6]utt_slope_b1!B3,3)</f>
         <v>MYN</v>
       </c>
       <c r="C13" s="17">
-        <f>[2]slope_b1!C3</f>
-        <v>3.54</v>
+        <f>[6]utt_slope_b1!C3</f>
+        <v>3.3940000000000001</v>
       </c>
       <c r="D13" s="17">
-        <f>[2]slope_b1!D3</f>
-        <v>0.874</v>
+        <f>[6]utt_slope_b1!D3</f>
+        <v>0.8</v>
       </c>
       <c r="E13" s="17">
-        <f>[2]slope_b1!E3</f>
-        <v>1.827</v>
+        <f>[6]utt_slope_b1!E3</f>
+        <v>1.825</v>
       </c>
       <c r="F13" s="17">
-        <f>[2]slope_b1!F3</f>
-        <v>5.2530000000000001</v>
+        <f>[6]utt_slope_b1!F3</f>
+        <v>4.9630000000000001</v>
       </c>
       <c r="G13" s="17">
-        <f>[2]slope_b1!G3</f>
-        <v>4.05</v>
+        <f>[6]utt_slope_b1!G3</f>
+        <v>4.24</v>
       </c>
       <c r="H13" s="45">
-        <f>[2]slope_b1!H3</f>
-        <v>10.01</v>
+        <f>[6]utt_slope_b1!H3</f>
+        <v>10.02</v>
       </c>
       <c r="I13" s="18">
-        <f>[2]slope_b1!I3</f>
-        <v>2.3E-3</v>
+        <f>[6]utt_slope_b1!I3</f>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="J13" s="19">
-        <f>[2]slope_b1!J3</f>
-        <v>9.2999999999999992E-3</v>
+        <f>[6]utt_slope_b1!J3</f>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="K13" s="16" t="str">
-        <f>[2]slope_b1!K3</f>
+        <f>[6]utt_slope_b1!K3</f>
         <v>p&lt;0.01</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="str">
-        <f>RIGHT([2]slope_b1!A4,3)</f>
+        <f>RIGHT([6]utt_slope_b1!A4,3)</f>
         <v>MDC</v>
       </c>
       <c r="B14" s="17" t="str">
-        <f>RIGHT([2]slope_b1!B4,3)</f>
+        <f>RIGHT([6]utt_slope_b1!B4,3)</f>
         <v>MDQ</v>
       </c>
       <c r="C14" s="17">
-        <f>[2]slope_b1!C4</f>
-        <v>6.516</v>
+        <f>[6]utt_slope_b1!C4</f>
+        <v>6.38</v>
       </c>
       <c r="D14" s="17">
-        <f>[2]slope_b1!D4</f>
-        <v>1.131</v>
+        <f>[6]utt_slope_b1!D4</f>
+        <v>1.1180000000000001</v>
       </c>
       <c r="E14" s="17">
-        <f>[2]slope_b1!E4</f>
-        <v>4.2990000000000004</v>
+        <f>[6]utt_slope_b1!E4</f>
+        <v>4.1890000000000001</v>
       </c>
       <c r="F14" s="17">
-        <f>[2]slope_b1!F4</f>
-        <v>8.7330000000000005</v>
+        <f>[6]utt_slope_b1!F4</f>
+        <v>8.57</v>
       </c>
       <c r="G14" s="17">
-        <f>[2]slope_b1!G4</f>
-        <v>5.7610000000000001</v>
+        <f>[6]utt_slope_b1!G4</f>
+        <v>5.7089999999999996</v>
       </c>
       <c r="H14" s="45">
-        <f>[2]slope_b1!H4</f>
-        <v>10.09</v>
+        <f>[6]utt_slope_b1!H4</f>
+        <v>10.119999999999999</v>
       </c>
       <c r="I14" s="18">
-        <f>[2]slope_b1!I4</f>
-        <v>1.7642999999999999E-4</v>
+        <f>[6]utt_slope_b1!I4</f>
+        <v>1.8699999999999999E-4</v>
       </c>
       <c r="J14" s="19">
-        <f>[2]slope_b1!J4</f>
-        <v>7.0600000000000003E-4</v>
+        <f>[6]utt_slope_b1!J4</f>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="K14" s="16" t="str">
-        <f>[2]slope_b1!K4</f>
+        <f>[6]utt_slope_b1!K4</f>
         <v>p&lt;0.001</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="str">
-        <f>RIGHT([2]slope_b1!A5,3)</f>
+        <f>RIGHT([6]utt_slope_b1!A5,3)</f>
         <v>MWH</v>
       </c>
       <c r="B15" s="17" t="str">
-        <f>RIGHT([2]slope_b1!B5,3)</f>
+        <f>RIGHT([6]utt_slope_b1!B5,3)</f>
         <v>MYN</v>
       </c>
       <c r="C15" s="17">
-        <f>[2]slope_b1!C5</f>
-        <v>5.9640000000000004</v>
+        <f>[6]utt_slope_b1!C5</f>
+        <v>5.4219999999999997</v>
       </c>
       <c r="D15" s="17">
-        <f>[2]slope_b1!D5</f>
-        <v>1.417</v>
+        <f>[6]utt_slope_b1!D5</f>
+        <v>1.4370000000000001</v>
       </c>
       <c r="E15" s="17">
-        <f>[2]slope_b1!E5</f>
-        <v>3.1859999999999999</v>
+        <f>[6]utt_slope_b1!E5</f>
+        <v>2.6059999999999999</v>
       </c>
       <c r="F15" s="17">
-        <f>[2]slope_b1!F5</f>
-        <v>8.7420000000000009</v>
+        <f>[6]utt_slope_b1!F5</f>
+        <v>8.2379999999999995</v>
       </c>
       <c r="G15" s="17">
-        <f>[2]slope_b1!G5</f>
-        <v>4.2080000000000002</v>
+        <f>[6]utt_slope_b1!G5</f>
+        <v>3.7730000000000001</v>
       </c>
       <c r="H15" s="45">
-        <f>[2]slope_b1!H5</f>
-        <v>10.01</v>
+        <f>[6]utt_slope_b1!H5</f>
+        <v>10.26</v>
       </c>
       <c r="I15" s="18">
-        <f>[2]slope_b1!I5</f>
-        <v>1.8E-3</v>
+        <f>[6]utt_slope_b1!I5</f>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="J15" s="19">
-        <f>[2]slope_b1!J5</f>
-        <v>7.1999999999999998E-3</v>
+        <f>[6]utt_slope_b1!J5</f>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="K15" s="16" t="str">
-        <f>[2]slope_b1!K5</f>
+        <f>[6]utt_slope_b1!K5</f>
         <v>p&lt;0.01</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="str">
-        <f>RIGHT([2]slope_b1!A6,3)</f>
+        <f>RIGHT([6]utt_slope_b1!A6,3)</f>
         <v>MWH</v>
       </c>
       <c r="B16" s="17" t="str">
-        <f>RIGHT([2]slope_b1!B6,3)</f>
+        <f>RIGHT([6]utt_slope_b1!B6,3)</f>
         <v>MDQ</v>
       </c>
       <c r="C16" s="17">
-        <f>[2]slope_b1!C6</f>
-        <v>8.94</v>
+        <f>[6]utt_slope_b1!C6</f>
+        <v>8.407</v>
       </c>
       <c r="D16" s="17">
-        <f>[2]slope_b1!D6</f>
-        <v>1.7509999999999999</v>
+        <f>[6]utt_slope_b1!D6</f>
+        <v>1.796</v>
       </c>
       <c r="E16" s="17">
-        <f>[2]slope_b1!E6</f>
-        <v>5.508</v>
+        <f>[6]utt_slope_b1!E6</f>
+        <v>4.8860000000000001</v>
       </c>
       <c r="F16" s="17">
-        <f>[2]slope_b1!F6</f>
-        <v>12.372</v>
+        <f>[6]utt_slope_b1!F6</f>
+        <v>11.928000000000001</v>
       </c>
       <c r="G16" s="17">
-        <f>[2]slope_b1!G6</f>
-        <v>5.1050000000000004</v>
+        <f>[6]utt_slope_b1!G6</f>
+        <v>4.68</v>
       </c>
       <c r="H16" s="45">
-        <f>[2]slope_b1!H6</f>
-        <v>10.02</v>
+        <f>[6]utt_slope_b1!H6</f>
+        <v>10.199999999999999</v>
       </c>
       <c r="I16" s="18">
-        <f>[2]slope_b1!I6</f>
-        <v>4.5785999999999998E-4</v>
+        <f>[6]utt_slope_b1!I6</f>
+        <v>8.2200000000000003E-4</v>
       </c>
       <c r="J16" s="19">
-        <f>[2]slope_b1!J6</f>
-        <v>1.8E-3</v>
+        <f>[6]utt_slope_b1!J6</f>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="K16" s="16" t="str">
-        <f>[2]slope_b1!K6</f>
+        <f>[6]utt_slope_b1!K6</f>
         <v>p&lt;0.01</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="41" t="str">
-        <f>RIGHT([2]slope_b1!A7,3)</f>
+        <f>RIGHT([6]utt_slope_b1!A7,3)</f>
         <v>MYN</v>
       </c>
       <c r="B17" s="42" t="str">
-        <f>RIGHT([2]slope_b1!B7,3)</f>
+        <f>RIGHT([6]utt_slope_b1!B7,3)</f>
         <v>MDQ</v>
       </c>
       <c r="C17" s="42">
-        <f>[2]slope_b1!C7</f>
-        <v>2.976</v>
+        <f>[6]utt_slope_b1!C7</f>
+        <v>2.9849999999999999</v>
       </c>
       <c r="D17" s="42">
-        <f>[2]slope_b1!D7</f>
-        <v>0.79900000000000004</v>
+        <f>[6]utt_slope_b1!D7</f>
+        <v>0.876</v>
       </c>
       <c r="E17" s="42">
-        <f>[2]slope_b1!E7</f>
-        <v>1.411</v>
+        <f>[6]utt_slope_b1!E7</f>
+        <v>1.268</v>
       </c>
       <c r="F17" s="42">
-        <f>[2]slope_b1!F7</f>
-        <v>4.5419999999999998</v>
+        <f>[6]utt_slope_b1!F7</f>
+        <v>4.7030000000000003</v>
       </c>
       <c r="G17" s="42">
-        <f>[2]slope_b1!G7</f>
-        <v>3.726</v>
+        <f>[6]utt_slope_b1!G7</f>
+        <v>3.4060000000000001</v>
       </c>
       <c r="H17" s="46">
-        <f>[2]slope_b1!H7</f>
-        <v>9.8800000000000008</v>
+        <f>[6]utt_slope_b1!H7</f>
+        <v>9.83</v>
       </c>
       <c r="I17" s="43">
-        <f>[2]slope_b1!I7</f>
-        <v>4.0000000000000001E-3</v>
+        <f>[6]utt_slope_b1!I7</f>
+        <v>6.8999999999999999E-3</v>
       </c>
       <c r="J17" s="47">
-        <f>[2]slope_b1!J7</f>
-        <v>1.61E-2</v>
+        <f>[6]utt_slope_b1!J7</f>
+        <v>1.18E-2</v>
       </c>
       <c r="K17" s="41" t="str">
-        <f>[2]slope_b1!K7</f>
+        <f>[6]utt_slope_b1!K7</f>
         <v>p&lt;0.05</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J17">
-    <cfRule type="containsText" dxfId="13" priority="108" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
+    <cfRule type="containsText" dxfId="112" priority="108" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.001",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="109" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
+    <cfRule type="containsText" dxfId="111" priority="109" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.01",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="110" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
+    <cfRule type="containsText" dxfId="110" priority="110" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.05",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="111" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
+    <cfRule type="containsText" dxfId="109" priority="111" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.1",J17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="containsText" dxfId="9" priority="76" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
+    <cfRule type="containsText" dxfId="108" priority="76" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.001",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="77" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
+    <cfRule type="containsText" dxfId="107" priority="77" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.01",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="78" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
+    <cfRule type="containsText" dxfId="106" priority="78" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.05",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="79" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
+    <cfRule type="containsText" dxfId="105" priority="79" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.1",J17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:K17">
-    <cfRule type="cellIs" dxfId="5" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="59" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K8">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J8 I12:J17">
-    <cfRule type="cellIs" dxfId="3" priority="80" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="80" stopIfTrue="1" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="81" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="81" stopIfTrue="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="82" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="82" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="83" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="83" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>